<commit_message>
update dataframes to list of lists
</commit_message>
<xml_diff>
--- a/data-raw/finance_lovs.xlsx
+++ b/data-raw/finance_lovs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="51">
   <si>
     <t>machine_name</t>
   </si>
@@ -150,13 +150,28 @@
     <t>Survey(Microdata)</t>
   </si>
   <si>
-    <t>Microdata</t>
-  </si>
-  <si>
     <t>field_license_wbddh</t>
   </si>
   <si>
     <t>Creative Commons Attribution 4.0</t>
+  </si>
+  <si>
+    <t>field_granularity_list</t>
+  </si>
+  <si>
+    <t>National</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Sub-national</t>
+  </si>
+  <si>
+    <t>Regional</t>
+  </si>
+  <si>
+    <t>Subnational</t>
   </si>
 </sst>
 </file>
@@ -1006,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,35 +1123,35 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1305,21 +1320,21 @@
         <v>32</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1327,10 +1342,10 @@
         <v>37</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1338,10 +1353,10 @@
         <v>37</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1349,21 +1364,65 @@
         <v>37</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>42</v>
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" t="s">
+        <v>39</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with data_type field as constant val
</commit_message>
<xml_diff>
--- a/data-raw/finance_lovs.xlsx
+++ b/data-raw/finance_lovs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="51">
   <si>
     <t>machine_name</t>
   </si>
@@ -1021,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1331,7 +1331,7 @@
         <v>37</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>39</v>
@@ -1342,10 +1342,10 @@
         <v>37</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1353,7 +1353,7 @@
         <v>37</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>39</v>
@@ -1364,18 +1364,18 @@
         <v>37</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>45</v>
-      </c>
-      <c r="B32" t="s">
-        <v>39</v>
+      <c r="A32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>39</v>
@@ -1386,10 +1386,10 @@
         <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1397,10 +1397,10 @@
         <v>45</v>
       </c>
       <c r="B34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1408,10 +1408,10 @@
         <v>45</v>
       </c>
       <c r="B35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1419,9 +1419,20 @@
         <v>45</v>
       </c>
       <c r="B36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>